<commit_message>
bug fixes in fixtures update script
</commit_message>
<xml_diff>
--- a/dimagi/samples/digitalgreen-ethiopia/digitalgreen-ethiopia_abezu_fixtures.xlsx
+++ b/dimagi/samples/digitalgreen-ethiopia/digitalgreen-ethiopia_abezu_fixtures.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="71">
   <si>
     <t>name</t>
   </si>
@@ -76,7 +76,160 @@
     <t>group 1</t>
   </si>
   <si>
+    <t>17583</t>
+  </si>
+  <si>
+    <t>Patimatla</t>
+  </si>
+  <si>
+    <t>abezu</t>
+  </si>
+  <si>
+    <t>18932</t>
+  </si>
+  <si>
+    <t>Sangam (Simra)</t>
+  </si>
+  <si>
     <t>field: village_id</t>
+  </si>
+  <si>
+    <t>6003</t>
+  </si>
+  <si>
+    <t>M.Narsaiah (CA)</t>
+  </si>
+  <si>
+    <t>7906</t>
+  </si>
+  <si>
+    <t>Sohan Sah</t>
+  </si>
+  <si>
+    <t>70844</t>
+  </si>
+  <si>
+    <t>Adarsha Mahila</t>
+  </si>
+  <si>
+    <t>70845</t>
+  </si>
+  <si>
+    <t>Bharathmatha</t>
+  </si>
+  <si>
+    <t>70846</t>
+  </si>
+  <si>
+    <t>Deevena</t>
+  </si>
+  <si>
+    <t>70847</t>
+  </si>
+  <si>
+    <t>Jhansi</t>
+  </si>
+  <si>
+    <t>70848</t>
+  </si>
+  <si>
+    <t>Kanakadurga</t>
+  </si>
+  <si>
+    <t>70849</t>
+  </si>
+  <si>
+    <t>Mahalaxmi</t>
+  </si>
+  <si>
+    <t>70850</t>
+  </si>
+  <si>
+    <t>Mallikarjuna</t>
+  </si>
+  <si>
+    <t>70851</t>
+  </si>
+  <si>
+    <t>Thelugu Mahila</t>
+  </si>
+  <si>
+    <t>70852</t>
+  </si>
+  <si>
+    <t>Sri Laxmi Durga</t>
+  </si>
+  <si>
+    <t>70853</t>
+  </si>
+  <si>
+    <t>Sri Rama</t>
+  </si>
+  <si>
+    <t>78952</t>
+  </si>
+  <si>
+    <t>Sharda SHG</t>
+  </si>
+  <si>
+    <t>78953</t>
+  </si>
+  <si>
+    <t>Anju</t>
+  </si>
+  <si>
+    <t>78954</t>
+  </si>
+  <si>
+    <t>Eklakhiya</t>
+  </si>
+  <si>
+    <t>78955</t>
+  </si>
+  <si>
+    <t>Gausiya</t>
+  </si>
+  <si>
+    <t>78956</t>
+  </si>
+  <si>
+    <t>Sita</t>
+  </si>
+  <si>
+    <t>78957</t>
+  </si>
+  <si>
+    <t>Madarsa</t>
+  </si>
+  <si>
+    <t>78958</t>
+  </si>
+  <si>
+    <t>Bhawani</t>
+  </si>
+  <si>
+    <t>78959</t>
+  </si>
+  <si>
+    <t>Jyoti</t>
+  </si>
+  <si>
+    <t>78960</t>
+  </si>
+  <si>
+    <t>Chameli</t>
+  </si>
+  <si>
+    <t>78961</t>
+  </si>
+  <si>
+    <t>Tegiya</t>
+  </si>
+  <si>
+    <t>78962</t>
+  </si>
+  <si>
+    <t>Radha</t>
   </si>
 </sst>
 </file>
@@ -489,7 +642,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -512,6 +665,28 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -519,7 +694,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -533,7 +708,7 @@
         <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -543,6 +718,34 @@
       </c>
       <c r="F1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -552,7 +755,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -566,7 +769,7 @@
         <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
@@ -576,6 +779,300 @@
       </c>
       <c r="F1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>